<commit_message>
Final edits - code cleanup
</commit_message>
<xml_diff>
--- a/RSA/data/Word_Data_race.xlsx
+++ b/RSA/data/Word_Data_race.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reem/Desktop/Research/DoubleHardMulticlass-Yolanda/Unequal_Representations/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reem/Desktop/Debiasing/RSA/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDD89578-51C4-2E42-A3DE-DA74534407CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B706079B-AA12-CE46-A70B-D0A5EF354D9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16720" yWindow="500" windowWidth="16880" windowHeight="16940" activeTab="2" xr2:uid="{09597D4B-E890-7544-9ACE-E2391760C702}"/>
+    <workbookView xWindow="1780" yWindow="500" windowWidth="30820" windowHeight="17580" xr2:uid="{09597D4B-E890-7544-9ACE-E2391760C702}"/>
   </bookViews>
   <sheets>
     <sheet name="White_Concept" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="30">
   <si>
     <t>manager</t>
   </si>
@@ -56,9 +56,6 @@
     <t>laborer</t>
   </si>
   <si>
-    <t>teacher</t>
-  </si>
-  <si>
     <t>slave</t>
   </si>
   <si>
@@ -77,87 +74,12 @@
     <t>Black_Concept</t>
   </si>
   <si>
-    <t>Jamaica</t>
-  </si>
-  <si>
-    <t>Haiti</t>
-  </si>
-  <si>
-    <t>Nigeria</t>
-  </si>
-  <si>
-    <t>Ethiopia</t>
-  </si>
-  <si>
-    <t>Somalia</t>
-  </si>
-  <si>
-    <t>Ghana</t>
-  </si>
-  <si>
-    <t>Asian_Roles</t>
-  </si>
-  <si>
-    <t>Black_Roles</t>
-  </si>
-  <si>
     <t>Asian_Concept</t>
   </si>
   <si>
-    <t>China</t>
-  </si>
-  <si>
-    <t>Asia</t>
-  </si>
-  <si>
-    <t>Tokyo</t>
-  </si>
-  <si>
-    <t>Japan</t>
-  </si>
-  <si>
-    <t>Hong Kong</t>
-  </si>
-  <si>
-    <t>South Korea</t>
-  </si>
-  <si>
-    <t>Singapore</t>
-  </si>
-  <si>
-    <t>Russia</t>
-  </si>
-  <si>
-    <t>America</t>
-  </si>
-  <si>
-    <t>England</t>
-  </si>
-  <si>
-    <t>Unite States</t>
-  </si>
-  <si>
     <t>White_Concept</t>
   </si>
   <si>
-    <t>White_Roles</t>
-  </si>
-  <si>
-    <t>Canada</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Australia </t>
-  </si>
-  <si>
-    <t>France</t>
-  </si>
-  <si>
-    <t>Germany</t>
-  </si>
-  <si>
-    <t>Europe</t>
-  </si>
-  <si>
     <t>black</t>
   </si>
   <si>
@@ -185,7 +107,16 @@
     <t>europe</t>
   </si>
   <si>
-    <t>america</t>
+    <t>White_Stereotypes</t>
+  </si>
+  <si>
+    <t>Asian_Stereotypes</t>
+  </si>
+  <si>
+    <t>Black_Stereotypes</t>
+  </si>
+  <si>
+    <t>scientists</t>
   </si>
 </sst>
 </file>
@@ -544,34 +475,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0EEA030-3C83-CE4D-93EE-1BBEF920684B}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" zoomScale="142" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="1" max="1" width="19.5" customWidth="1"/>
+    <col min="2" max="2" width="21" customWidth="1"/>
     <col min="3" max="4" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -579,16 +510,13 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -596,81 +524,48 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>51</v>
-      </c>
-      <c r="F4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F10" t="s">
-        <v>32</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -680,38 +575,35 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D249510-1CC9-BF4F-A202-699D9CF92948}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="G16" sqref="G3:G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.1640625" customWidth="1"/>
-    <col min="2" max="2" width="16.83203125" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="1" max="1" width="24" customWidth="1"/>
+    <col min="2" max="2" width="21" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" customWidth="1"/>
     <col min="4" max="4" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -719,16 +611,13 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -736,63 +625,48 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>46</v>
-      </c>
-      <c r="F4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
         <v>13</v>
       </c>
-      <c r="F5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F7" t="s">
-        <v>30</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -804,33 +678,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03674D3D-4F58-654B-9C88-D43E70EA1BC3}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView zoomScale="214" workbookViewId="0">
+      <selection activeCell="F11" sqref="F3:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" customWidth="1"/>
-    <col min="2" max="2" width="14.5" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" customWidth="1"/>
+    <col min="2" max="2" width="20.5" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
     <col min="4" max="4" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -841,13 +712,10 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -858,30 +726,24 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -889,13 +751,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
         <v>13</v>
-      </c>
-      <c r="F5" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -903,15 +762,12 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>